<commit_message>
Add Validation and Pricing panel tests and updated login
</commit_message>
<xml_diff>
--- a/src/test/java/TestData/TestData.xlsx
+++ b/src/test/java/TestData/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82692d6075d90582/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{49C853CF-0F75-4868-826C-7486A04B1F75}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C294AD49-9B81-4E05-9F82-E7EC03BE4F40}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{B8B0331D-AC97-453D-BB68-37A8ABA4D337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{ECFA3456-4D27-4291-8796-3E43C48B9295}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Email</t>
   </si>
@@ -48,6 +48,9 @@
   </si>
   <si>
     <t>5oe620cnnialx</t>
+  </si>
+  <si>
+    <t>vbznznxzx</t>
   </si>
 </sst>
 </file>
@@ -430,15 +433,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{152EADC7-7CB3-4285-A84D-6CD16A531F35}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.140625" customWidth="1"/>
     <col min="2" max="2" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -458,6 +461,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{77E464FB-37F6-49ED-9F1E-2FE4E06AEFD9}"/>

</xml_diff>